<commit_message>
one time run file
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/Qeetoto-Scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08ED9C7-E44E-B243-8E59-AA625C7021D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F8979B-231C-A946-A78C-3B711B1AC42F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,8 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -396,7 +397,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -451,8 +452,14 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+    </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>

</xml_diff>

<commit_message>
nexyDay and Prevday func not working
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -15,15 +15,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt formatCode="yyyy\-mm\-dd" numFmtId="164"/>
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="165"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -47,10 +55,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -348,87 +358,86 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="20.33203125"/>
-    <col customWidth="1" max="2" min="2" width="12.1640625"/>
-    <col customWidth="1" max="3" min="3" width="10.33203125"/>
-    <col customWidth="1" max="4" min="4" width="14.1640625"/>
-    <col customWidth="1" max="5" min="5" width="15.6640625"/>
-    <col customWidth="1" max="6" min="6" width="11"/>
-    <col customWidth="1" max="7" min="7" width="12.1640625"/>
-    <col customWidth="1" max="8" min="8" width="8"/>
-    <col customWidth="1" max="9" min="9" width="7.6640625"/>
-    <col customWidth="1" max="10" min="10" width="7"/>
+    <col customWidth="1" max="2" min="2" width="7.5"/>
+    <col customWidth="1" max="3" min="3" width="13"/>
+    <col customWidth="1" max="4" min="4" width="7.1640625"/>
+    <col customWidth="1" max="5" min="5" width="7.33203125"/>
+    <col customWidth="1" max="7" min="6" width="5"/>
+    <col customWidth="1" max="8" min="8" width="11"/>
+    <col customWidth="1" max="9" min="9" width="10"/>
+    <col customWidth="1" max="10" min="10" width="11.1640625"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Operator Name/Date</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+    <row customHeight="1" ht="16" r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Operator Name</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Provider Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Game Name</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Number Of Plays</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Difference To Mean</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Average Stake</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Unique Players</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>Turnover</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>Returns</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>Margin</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>43938</v>
+      <c r="A2" s="3" t="n">
+        <v>43447</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>William Hill Riga</t>
+          <t>Bet Victor</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -442,25 +451,31 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>1900</v>
       </c>
       <c r="E3" t="n">
-        <v>100</v>
+        <v>7302.52</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>20.17</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.15</v>
+        <v>56</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -469,25 +484,31 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="H4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.15</v>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>43938</v>
+      <c r="A5" s="3" t="n">
+        <v>43448</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>William Hill Riga</t>
+          <t>Bet Victor</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -501,57 +522,624 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>1900</v>
       </c>
       <c r="E6" t="n">
-        <v>100</v>
+        <v>7302.52</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5</v>
+        <v>20.17</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.15</v>
+        <v>56</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.15</v>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n"/>
+      <c r="A8" s="3" t="n">
+        <v>43449</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Bet Victor</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Qeetoto</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Texas HedgeEm</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1900</v>
+      </c>
+      <c r="E9" t="n">
+        <v>7302.52</v>
+      </c>
+      <c r="F9" t="n">
+        <v>20.17</v>
+      </c>
+      <c r="G9" t="n">
+        <v>56</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n"/>
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n"/>
+      <c r="A11" s="3" t="n">
+        <v>43450</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Bet Victor</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Qeetoto</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Texas HedgeEm</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1900</v>
+      </c>
+      <c r="E12" t="n">
+        <v>7302.52</v>
+      </c>
+      <c r="F12" t="n">
+        <v>20.17</v>
+      </c>
+      <c r="G12" t="n">
+        <v>56</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>43451</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Bet Victor</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Qeetoto</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Texas HedgeEm</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1900</v>
+      </c>
+      <c r="E15" t="n">
+        <v>7302.52</v>
+      </c>
+      <c r="F15" t="n">
+        <v>20.17</v>
+      </c>
+      <c r="G15" t="n">
+        <v>56</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>43452</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Bet Victor</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Qeetoto</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Texas HedgeEm</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1900</v>
+      </c>
+      <c r="E18" t="n">
+        <v>7302.52</v>
+      </c>
+      <c r="F18" t="n">
+        <v>20.17</v>
+      </c>
+      <c r="G18" t="n">
+        <v>56</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Bet Victor</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Qeetoto</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Texas HedgeEm</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1900</v>
+      </c>
+      <c r="E21" t="n">
+        <v>7302.52</v>
+      </c>
+      <c r="F21" t="n">
+        <v>20.17</v>
+      </c>
+      <c r="G21" t="n">
+        <v>56</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>43454</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Bet Victor</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Qeetoto</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Texas HedgeEm</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1900</v>
+      </c>
+      <c r="E24" t="n">
+        <v>7302.52</v>
+      </c>
+      <c r="F24" t="n">
+        <v>20.17</v>
+      </c>
+      <c r="G24" t="n">
+        <v>56</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>38,323.60</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>37,317.61</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>1,005.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="n">
+        <v>43462</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="n">
+        <v>43463</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="n">
+        <v>43464</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="n">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="n"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="16" r="42"/>
+    <row r="43">
+      <c r="A43" s="3" t="n"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="n"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="n"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="n"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="n"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="n"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="n"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="n"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="n"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="n"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="n"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="n"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="n"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="n"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="n"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="n"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="n"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="n"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="3" t="n"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="3" t="n"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="3" t="n"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="3" t="n"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="3" t="n"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="3" t="n"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="3" t="n"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="3" t="n"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="3" t="n"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="3" t="n"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="3" t="n"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="3" t="n"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="3" t="n"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="3" t="n"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="3" t="n"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="3" t="n"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="3" t="n"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="3" t="n"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>